<commit_message>
Modifying naming scheme on database schema.
</commit_message>
<xml_diff>
--- a/Resources/Presentation 3/csci-4712-db-schema.xlsx
+++ b/Resources/Presentation 3/csci-4712-db-schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\csci-4712-senior-capstone\Resources\Presentation 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,9 +89,6 @@
     <t>Title : VARCHAR(140)</t>
   </si>
   <si>
-    <t>TimeFrame : DATETIME</t>
-  </si>
-  <si>
     <t>Category : VARCHAR(24)</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Title:VARCHAR(140)</t>
+  </si>
+  <si>
+    <t>Timeframe : DATETIME</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,22 +572,22 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -676,19 +676,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -741,25 +741,25 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
         <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -806,22 +806,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -841,25 +841,25 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="s">
         <v>28</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Creating dummy page for Create Dpeartment and Create Employee - with proper structure for expansion later
</commit_message>
<xml_diff>
--- a/Resources/Presentation 3/csci-4712-db-schema.xlsx
+++ b/Resources/Presentation 3/csci-4712-db-schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\csci-4712-senior-capstone\Resources\Presentation 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Documents\GitHub\csci-4712-senior-capstone\Resources\Presentation 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>John</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Timeframe : DATETIME</t>
+  </si>
+  <si>
+    <t>Email:Varchar(32)</t>
   </si>
 </sst>
 </file>
@@ -550,21 +553,21 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="4" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -589,8 +592,11 @@
       <c r="H1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -616,7 +622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -642,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -668,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -691,7 +697,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -705,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -719,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -733,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -762,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -776,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -790,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -804,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -824,22 +830,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -862,17 +868,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>

</xml_diff>